<commit_message>
Added the Shipment_Overview, Shipment_All, Shipment_Defaulted etc. procedures
</commit_message>
<xml_diff>
--- a/EvalautionStatus.xlsx
+++ b/EvalautionStatus.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="23220" windowHeight="10665"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="23220" windowHeight="10660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -104,10 +108,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,8 +150,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -140,7 +168,15 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -443,65 +479,65 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -509,7 +545,7 @@
         <v>41469</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -535,7 +571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -561,7 +597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -587,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -613,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -639,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -665,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -675,7 +711,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -685,7 +721,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -695,7 +731,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -705,7 +741,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -715,7 +751,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -725,7 +761,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -733,7 +769,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -741,17 +777,17 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -762,7 +798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="B31" t="s">
         <v>6</v>
       </c>
@@ -770,7 +806,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="B32" t="s">
         <v>7</v>
       </c>
@@ -778,7 +814,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3">
       <c r="B33" t="s">
         <v>8</v>
       </c>
@@ -788,6 +824,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -797,9 +839,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -809,8 +856,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>